<commit_message>
added heartbeat with heapless crate and aes in C
</commit_message>
<xml_diff>
--- a/new_updated_values.xlsx
+++ b/new_updated_values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KumarAnkita\Documents\trying_on_win\masterarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760D6A40-150A-484E-81CD-2BDD3D629DD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90428A4-4090-4C14-ACFC-6E21A760B61E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6930" xr2:uid="{17B47634-282A-46EE-8CBE-C662B8DD9DDC}"/>
   </bookViews>
@@ -168,16 +168,16 @@
     <t>aad_round_key</t>
   </si>
   <si>
-    <t>Rust NVM</t>
-  </si>
-  <si>
-    <t>C NVM</t>
-  </si>
-  <si>
     <t>C NVM without addroundkey and keyexpansion</t>
   </si>
   <si>
     <t>Sum without constant Rcon and Sbox and no key expansion</t>
+  </si>
+  <si>
+    <t>Rust</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -343,12 +343,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="de-DE" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>CPU Cycles with NVM Size</a:t>
             </a:r>
-            <a:endParaRPr lang="de-DE">
+            <a:endParaRPr lang="de-DE" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -423,9 +423,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$J$5:$J$8</c:f>
+              <c:f>Sheet1!$J$5:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>O2</c:v>
                 </c:pt>
@@ -434,9 +434,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Os</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -450,10 +447,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$M$5:$M$8</c:f>
+              <c:f>Sheet1!$M$5:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3338</c:v>
                 </c:pt>
@@ -462,9 +459,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6655</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8534</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -508,9 +502,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$J$5:$J$8</c:f>
+              <c:f>Sheet1!$J$5:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>O2</c:v>
                 </c:pt>
@@ -519,9 +513,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Os</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -535,10 +526,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$N$5:$N$8</c:f>
+              <c:f>Sheet1!$N$5:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>5987</c:v>
                 </c:pt>
@@ -547,9 +538,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7071</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,7 +557,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rust NVM</c:v>
+                  <c:v>Rust</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -593,9 +581,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$J$5:$J$8</c:f>
+              <c:f>Sheet1!$J$5:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>O2</c:v>
                 </c:pt>
@@ -604,9 +592,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Os</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -620,10 +605,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$K$5:$K$8</c:f>
+              <c:f>Sheet1!$K$5:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1385</c:v>
                 </c:pt>
@@ -632,9 +617,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>456</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,7 +636,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C NVM</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -678,9 +660,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$J$5:$J$8</c:f>
+              <c:f>Sheet1!$J$5:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>O2</c:v>
                 </c:pt>
@@ -689,9 +671,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Os</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -705,10 +684,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$L$5:$L$8</c:f>
+              <c:f>Sheet1!$L$5:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1090</c:v>
                 </c:pt>
@@ -717,9 +696,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>394</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>348</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1083,7 +1059,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>NVM Size</a:t>
+              <a:t>NVM Size vs Optimisation levels</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1132,7 +1108,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rust NVM</c:v>
+                  <c:v>Rust</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1230,7 +1206,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C NVM</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2758,16 +2734,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>160337</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>87313</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>163511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1587</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1586</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3666,8 +3642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663F724C-4613-4E36-9F5C-AC929F1452D5}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3703,10 +3679,10 @@
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>37</v>
@@ -3967,7 +3943,7 @@
         <v>256</v>
       </c>
       <c r="L13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -4037,7 +4013,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L17">
         <v>1250</v>

</xml_diff>